<commit_message>
[ADD] Added pipeline to test symbolic dynamic models
</commit_message>
<xml_diff>
--- a/Documents/20220314_experiments_schedule.xlsx
+++ b/Documents/20220314_experiments_schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\ACL_LABisca\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\OneDrive\Desktop\Polimi\Automation and Control Laboratory\ACL_LABisca\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43FB5B9-F7F6-41A7-AC5A-8345D943115A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF08DB-85B4-43AF-A2F3-6D4F62AFD59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAF9A911-7350-46AF-A290-CDA872147E99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FAF9A911-7350-46AF-A290-CDA872147E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -122,6 +122,47 @@
   </si>
   <si>
     <t>Find K of the cable</t>
+  </si>
+  <si>
+    <t>PD controller test step response</t>
+  </si>
+  <si>
+    <t>Control the system via the PD controller and set the theta
+reference to a constant value</t>
+  </si>
+  <si>
+    <t>Check static performance of the
+controller</t>
+  </si>
+  <si>
+    <t>PD controller test dynamic
+response</t>
+  </si>
+  <si>
+    <t>Control the system via the PD controller and set the theta
+reference to a sinusoid slower than the cutting frequency</t>
+  </si>
+  <si>
+    <t>Check dynamic performance of the
+controller</t>
+  </si>
+  <si>
+    <t>Paolo</t>
+  </si>
+  <si>
+    <t>PID controller test step response</t>
+  </si>
+  <si>
+    <t>PID controller test dynamic
+response</t>
+  </si>
+  <si>
+    <t>Control the system via the PID controller and set the theta
+reference to a constant value</t>
+  </si>
+  <si>
+    <t>Control the system via the PID controller and set the theta
+reference to a sinusoid slower than the cutting frequency</t>
   </si>
 </sst>
 </file>
@@ -684,21 +725,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1ABF9A4-757F-4E62-8F7C-82A772F2FFE1}">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -718,7 +759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>1</v>
       </c>
@@ -736,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>2</v>
       </c>
@@ -754,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -772,7 +813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14">
         <v>4</v>
       </c>
@@ -786,7 +827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -804,7 +845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>6</v>
       </c>
@@ -818,7 +859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -836,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>8</v>
       </c>
@@ -850,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -868,7 +909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
         <v>10</v>
       </c>
@@ -886,47 +927,79 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>11</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="14">
         <v>12</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="17"/>
+      <c r="C15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>13</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B17" s="14">
         <v>14</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="17"/>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" s="6"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -936,7 +1009,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="14">
         <v>16</v>
       </c>
@@ -946,7 +1019,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="15">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
[ADD] Add robustness experiments
</commit_message>
<xml_diff>
--- a/Documents/20220314_experiments_schedule.xlsx
+++ b/Documents/20220314_experiments_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\OneDrive\Desktop\Polimi\Automation and Control Laboratory\ACL_LABisca\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescoceresetti/Documents/MATLAB/MATLAB 2019/ACL_LABisca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF08DB-85B4-43AF-A2F3-6D4F62AFD59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985F70DA-C8B7-F443-8230-DF14CAC29350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FAF9A911-7350-46AF-A290-CDA872147E99}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="14500" xr2:uid="{FAF9A911-7350-46AF-A290-CDA872147E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -147,9 +147,6 @@
 controller</t>
   </si>
   <si>
-    <t>Paolo</t>
-  </si>
-  <si>
     <t>PID controller test step response</t>
   </si>
   <si>
@@ -163,6 +160,29 @@
   <si>
     <t>Control the system via the PID controller and set the theta
 reference to a sinusoid slower than the cutting frequency</t>
+  </si>
+  <si>
+    <t>PD controller test robustness</t>
+  </si>
+  <si>
+    <t>PID controller test robustness</t>
+  </si>
+  <si>
+    <t>Control the system via the PD controller and set the theta
+reference to a constant value, when stable, slightly hit the pendulum to generate some oscillations</t>
+  </si>
+  <si>
+    <t>Control the system via the PID controller and set the theta
+reference to a constant value, when stable, slightly hit the pendulum to generate some oscillations</t>
+  </si>
+  <si>
+    <t>Check robustness of the controller</t>
+  </si>
+  <si>
+    <t>Cere</t>
+  </si>
+  <si>
+    <t>Pöl</t>
   </si>
 </sst>
 </file>
@@ -411,7 +431,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,7 +447,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,21 +745,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1ABF9A4-757F-4E62-8F7C-82A772F2FFE1}">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -759,7 +779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="13">
         <v>1</v>
       </c>
@@ -777,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="14">
         <v>2</v>
       </c>
@@ -795,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -813,7 +833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14">
         <v>4</v>
       </c>
@@ -827,7 +847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -845,7 +865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14">
         <v>6</v>
       </c>
@@ -859,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -877,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14">
         <v>8</v>
       </c>
@@ -891,7 +911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -909,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="14">
         <v>10</v>
       </c>
@@ -927,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="14">
         <v>11</v>
       </c>
@@ -942,10 +962,10 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" s="14">
         <v>12</v>
       </c>
@@ -960,66 +980,82 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>13</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="14">
         <v>14</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B18" s="14">
         <v>15</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="17"/>
+      <c r="C18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="14">
         <v>16</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="17"/>
+      <c r="C19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="15">
         <v>17</v>
       </c>

</xml_diff>